<commit_message>
Adding more power level values to CC adversaries
</commit_message>
<xml_diff>
--- a/CR Calculator.xlsx
+++ b/CR Calculator.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Projects\genesys-adversaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43170779-975F-4652-ADEA-15A8DE288E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0647E30D-E6C8-455D-8699-6374A55CDE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="3450" windowWidth="8850" windowHeight="9855" xr2:uid="{07AF5B8C-A12A-4A72-AD2C-DDE6A5BC5A52}"/>
+    <workbookView xWindow="9645" yWindow="9645" windowWidth="28770" windowHeight="11955" xr2:uid="{07AF5B8C-A12A-4A72-AD2C-DDE6A5BC5A52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>Name Characteristics Power Levels Examples</t>
   </si>
@@ -166,9 +165,6 @@
     <t>Terrifying</t>
   </si>
   <si>
-    <t>Ghostly</t>
-  </si>
-  <si>
     <t>Flyer</t>
   </si>
   <si>
@@ -179,6 +175,12 @@
   </si>
   <si>
     <t>Wounds over Brawn+8 (rivals) or Brawn+12 (nemeses)</t>
+  </si>
+  <si>
+    <t>Swarm</t>
+  </si>
+  <si>
+    <t>Ghostly/Demonic</t>
   </si>
 </sst>
 </file>
@@ -544,13 +546,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC15AD63-1188-4210-A173-3F9DA32F5291}">
-  <dimension ref="A1:M67"/>
+  <dimension ref="A1:M86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -680,31 +685,31 @@
         <v>5</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E20">
         <v>3</v>
       </c>
       <c r="F20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H20" s="1">
         <f>VLOOKUP(B20+C20,$L$19:$M$27,2,TRUE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I20" s="1">
         <f>VLOOKUP(F20+G20,$L$19:$M$27,2,TRUE)</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="J20" s="1">
         <f>VLOOKUP(E20+D20,$L$19:$M$27,2,TRUE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L20">
         <v>2</v>
@@ -742,11 +747,11 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H24">
         <f>VLOOKUP(B24,$L$32:$M$36,2,TRUE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24">
         <v>6</v>
@@ -773,15 +778,15 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B29">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H29">
-        <f>VLOOKUP(B29,$L$39:$M$43,2,TRUE)</f>
+        <f>VLOOKUP(B29,$L$39:$M$45,2,TRUE)</f>
         <v>1</v>
       </c>
     </row>
@@ -801,7 +806,7 @@
         <v>4</v>
       </c>
       <c r="I32">
-        <f>VLOOKUP(B32,$L$46:$M$48,2,TRUE)</f>
+        <f>VLOOKUP(B32,$L$52:$M$56,2,TRUE)</f>
         <v>0</v>
       </c>
       <c r="L32">
@@ -832,10 +837,10 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35">
-        <f>VLOOKUP(B35,$L$50:$M$53,2,TRUE)</f>
+        <f>VLOOKUP(B35,$L$69:$M$72,2,TRUE)</f>
         <v>0</v>
       </c>
       <c r="L35">
@@ -863,12 +868,12 @@
         <v>33</v>
       </c>
       <c r="B38">
-        <f>3+1+4+1</f>
-        <v>9</v>
+        <f>3+2+1</f>
+        <v>6</v>
       </c>
       <c r="H38">
         <f>_xlfn.FLOOR.MATH(B38/3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L38" t="s">
         <v>29</v>
@@ -882,7 +887,6 @@
         <v>34</v>
       </c>
       <c r="B39">
-        <f>0</f>
         <v>0</v>
       </c>
       <c r="I39">
@@ -901,12 +905,12 @@
         <v>35</v>
       </c>
       <c r="B40">
-        <f>4+3</f>
-        <v>7</v>
+        <f>2+1</f>
+        <v>3</v>
       </c>
       <c r="J40">
         <f>_xlfn.FLOOR.MATH(B40/3)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L40">
         <v>2</v>
@@ -944,61 +948,57 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B44">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H44">
-        <f>VLOOKUP(B44,$L$56:$M$67,2,TRUE)</f>
-        <v>1</v>
+        <f>VLOOKUP(B44,$L$75:$M$86,2,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="L44">
+        <v>35</v>
+      </c>
+      <c r="M44">
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L45" t="s">
-        <v>31</v>
-      </c>
-      <c r="M45" t="s">
-        <v>25</v>
+      <c r="L45">
+        <v>50</v>
+      </c>
+      <c r="M45">
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>39</v>
       </c>
-      <c r="L46">
-        <v>0</v>
-      </c>
-      <c r="M46">
-        <v>0</v>
-      </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47">
         <f>B47*2</f>
-        <v>0</v>
-      </c>
-      <c r="L47">
-        <v>5</v>
-      </c>
-      <c r="M47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L48">
-        <v>10</v>
-      </c>
-      <c r="M48">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L49" t="s">
-        <v>30</v>
-      </c>
-      <c r="M49" t="s">
-        <v>25</v>
+      <c r="A49" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <f>$B$51*1</f>
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -1006,7 +1006,7 @@
         <v>41</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -1016,12 +1016,6 @@
       </c>
       <c r="J50">
         <f>B50*2</f>
-        <v>2</v>
-      </c>
-      <c r="L50">
-        <v>0</v>
-      </c>
-      <c r="M50">
         <v>0</v>
       </c>
     </row>
@@ -1030,30 +1024,30 @@
         <v>42</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H51">
         <f>$B$51*1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I51">
         <f>$B$51*1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J51">
         <f>$B$51*1</f>
-        <v>1</v>
-      </c>
-      <c r="L51">
-        <v>1</v>
-      </c>
-      <c r="M51">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="L51" t="s">
+        <v>31</v>
+      </c>
+      <c r="M51" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -1070,15 +1064,15 @@
         <v>0</v>
       </c>
       <c r="L52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M52">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -1094,15 +1088,15 @@
         <v>0</v>
       </c>
       <c r="L53">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M53">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -1117,10 +1111,16 @@
         <f>B54*1</f>
         <v>0</v>
       </c>
+      <c r="L54">
+        <v>10</v>
+      </c>
+      <c r="M54">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -1135,52 +1135,33 @@
       <c r="J55">
         <v>0</v>
       </c>
-      <c r="L55" t="s">
-        <v>38</v>
+      <c r="L55">
+        <v>20</v>
+      </c>
+      <c r="M55">
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L56">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="M56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L57">
-        <v>5</v>
-      </c>
-      <c r="M57">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H58" s="2">
-        <f>MAX(SUM(H18:H54),1)</f>
-        <v>7</v>
+        <f>MAX(SUM(H18:H55),1)</f>
+        <v>9</v>
       </c>
       <c r="I58" s="2">
-        <f>MAX(SUM(I18:I54),1)</f>
-        <v>2</v>
+        <f>MAX(SUM(I18:I55),1)</f>
+        <v>1</v>
       </c>
       <c r="J58" s="2">
-        <f>MAX(SUM(J18:J54),1)</f>
-        <v>6</v>
-      </c>
-      <c r="L58">
-        <v>6</v>
-      </c>
-      <c r="M58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L59">
-        <v>7</v>
-      </c>
-      <c r="M59">
-        <v>0</v>
+        <f>MAX(SUM(J18:J55),1)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
@@ -1193,66 +1174,145 @@
       <c r="J60" t="s">
         <v>35</v>
       </c>
-      <c r="L60">
+    </row>
+    <row r="68" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L68" t="s">
+        <v>30</v>
+      </c>
+      <c r="M68" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L69">
+        <v>0</v>
+      </c>
+      <c r="M69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L70">
+        <v>1</v>
+      </c>
+      <c r="M70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L71">
+        <v>2</v>
+      </c>
+      <c r="M71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L72">
+        <v>4</v>
+      </c>
+      <c r="M72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L74" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="75" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L75">
+        <v>4</v>
+      </c>
+      <c r="M75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L76">
+        <v>5</v>
+      </c>
+      <c r="M76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L77">
+        <v>6</v>
+      </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L78">
+        <v>7</v>
+      </c>
+      <c r="M78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L79">
         <v>8</v>
       </c>
-      <c r="M60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L61">
+      <c r="M79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L80">
         <v>9</v>
       </c>
-      <c r="M61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L62">
+      <c r="M80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L81">
         <v>10</v>
       </c>
-      <c r="M62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L63">
+      <c r="M81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L82">
         <v>11</v>
       </c>
-      <c r="M63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L64">
+      <c r="M82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L83">
         <v>12</v>
       </c>
-      <c r="M64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L65">
+      <c r="M83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L84">
         <v>13</v>
       </c>
-      <c r="M65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L66">
+      <c r="M84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L85">
         <v>14</v>
       </c>
-      <c r="M66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L67">
+      <c r="M85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L86">
         <v>15</v>
       </c>
-      <c r="M67">
+      <c r="M86">
         <v>2</v>
       </c>
     </row>

</xml_diff>